<commit_message>
ideal school meal top preferences
</commit_message>
<xml_diff>
--- a/SurveyData/School_1b_2021.xlsx
+++ b/SurveyData/School_1b_2021.xlsx
@@ -7,8 +7,8 @@
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="Word_Freq_Q28" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="Sent_Freq_Q30" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="Freq_Q28" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Freq_Q30" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -2123,10 +2123,10 @@
         </is>
       </c>
       <c r="N3" t="n">
-        <v>52.14570617675781</v>
+        <v>52.1457061767578</v>
       </c>
       <c r="O3" t="n">
-        <v>-0.8802947998046875</v>
+        <v>-0.8802947998046881</v>
       </c>
       <c r="P3" t="inlineStr">
         <is>
@@ -2185,7 +2185,7 @@
       </c>
       <c r="BE3" t="inlineStr">
         <is>
-          <t>offer at least one portion of fresh fruit and vegetables everyday,offer mainly wholemeal carbohydrates (whole-grain bread, brown rice, or pasta for example)</t>
+          <t>offer at least one portion of fresh fruit and vegetables everyday,offer mainly wholemeal carbohydrates (whole-grain bread; brown rice; or pasta for example)</t>
         </is>
       </c>
       <c r="BH3" t="inlineStr">
@@ -2406,10 +2406,10 @@
         </is>
       </c>
       <c r="N4" t="n">
-        <v>52.14570617675781</v>
+        <v>52.1457061767578</v>
       </c>
       <c r="O4" t="n">
-        <v>-0.8802947998046875</v>
+        <v>-0.8802947998046881</v>
       </c>
       <c r="P4" t="inlineStr">
         <is>
@@ -2503,7 +2503,7 @@
       </c>
       <c r="BE4" t="inlineStr">
         <is>
-          <t>offer at least one portion of fresh fruit and vegetables everyday,offer mainly wholemeal carbohydrates (whole-grain bread, brown rice, or pasta for example),offer only high quality grass-fed meat options</t>
+          <t>offer at least one portion of fresh fruit and vegetables everyday,offer mainly wholemeal carbohydrates (whole-grain bread; brown rice; or pasta for example),offer only high quality grass-fed meat options</t>
         </is>
       </c>
       <c r="BG4" t="n">
@@ -2511,7 +2511,7 @@
       </c>
       <c r="BH4" t="inlineStr">
         <is>
-          <t>reduce high-carbon &amp; water footprint foods (meat and dairy, for example),minimise waste,contain locally sourced ingredients,contain organically sourced ingredients,contain  seasonally sourced ingredients,are cooked from scratch in the school kitchen,meet all dietary requirements,should be enjoyed by pupils,offer high quality grass-fed meat options</t>
+          <t>reduce high-carbon &amp; water footprint foods (meat and dairy; for example),minimise waste,contain locally sourced ingredients,contain organically sourced ingredients,contain  seasonally sourced ingredients,are cooked from scratch in the school kitchen,meet all dietary requirements,should be enjoyed by pupils,offer high quality grass-fed meat options</t>
         </is>
       </c>
       <c r="BJ4" t="n">
@@ -2740,7 +2740,7 @@
         </is>
       </c>
       <c r="N5" t="n">
-        <v>51.49639892578125</v>
+        <v>51.4963989257813</v>
       </c>
       <c r="O5" t="n">
         <v>-0.122406005859375</v>
@@ -2822,7 +2822,7 @@
       </c>
       <c r="BE5" t="inlineStr">
         <is>
-          <t>offer at least one portion of fresh fruit and vegetables everyday,are void of trans-fats* (artificially created fats used in the manufacture of foods to increase shelf life and the flavour-stability of foods. They are also often found in fast food, margarine, cakes and biscuits),offer added-sugar free days,offer mainly wholemeal carbohydrates (whole-grain bread, brown rice, or pasta for example),offer only high quality grass-fed meat options</t>
+          <t>offer at least one portion of fresh fruit and vegetables everyday,are void of trans-fats* (artificially created fats used in the manufacture of foods to increase shelf life and the flavour-stability of foods. They are also often found in fast food; margarine; cakes and biscuits),offer added-sugar free days,offer mainly wholemeal carbohydrates (whole-grain bread; brown rice; or pasta for example),offer only high quality grass-fed meat options</t>
         </is>
       </c>
       <c r="BG5" t="n">
@@ -2830,7 +2830,7 @@
       </c>
       <c r="BH5" t="inlineStr">
         <is>
-          <t>reduce high-carbon &amp; water footprint foods (meat and dairy, for example),minimise waste,contain locally sourced ingredients,contain organically sourced ingredients,contain  seasonally sourced ingredients,should be enjoyed by pupils,offer high quality grass-fed meat options</t>
+          <t>reduce high-carbon &amp; water footprint foods (meat and dairy; for example),minimise waste,contain locally sourced ingredients,contain organically sourced ingredients,contain  seasonally sourced ingredients,should be enjoyed by pupils,offer high quality grass-fed meat options</t>
         </is>
       </c>
       <c r="BJ5" t="n">
@@ -2963,10 +2963,10 @@
         </is>
       </c>
       <c r="N6" t="n">
-        <v>50.70179748535156</v>
+        <v>50.7017974853516</v>
       </c>
       <c r="O6" t="n">
-        <v>-3.534698486328125</v>
+        <v>-3.53469848632812</v>
       </c>
       <c r="P6" t="inlineStr">
         <is>
@@ -3063,7 +3063,7 @@
       </c>
       <c r="BH6" t="inlineStr">
         <is>
-          <t>reduce high-carbon &amp; water footprint foods (meat and dairy, for example),minimise waste,contain locally sourced ingredients,contain organically sourced ingredients,contain  seasonally sourced ingredients,meet all dietary requirements,should be enjoyed by pupils</t>
+          <t>reduce high-carbon &amp; water footprint foods (meat and dairy; for example),minimise waste,contain locally sourced ingredients,contain organically sourced ingredients,contain  seasonally sourced ingredients,meet all dietary requirements,should be enjoyed by pupils</t>
         </is>
       </c>
       <c r="BJ6" t="n">
@@ -3404,7 +3404,7 @@
       </c>
       <c r="BE7" t="inlineStr">
         <is>
-          <t>offer at least one portion of fresh fruit and vegetables everyday,are void of trans-fats* (artificially created fats used in the manufacture of foods to increase shelf life and the flavour-stability of foods. They are also often found in fast food, margarine, cakes and biscuits)</t>
+          <t>offer at least one portion of fresh fruit and vegetables everyday,are void of trans-fats* (artificially created fats used in the manufacture of foods to increase shelf life and the flavour-stability of foods. They are also often found in fast food; margarine; cakes and biscuits)</t>
         </is>
       </c>
       <c r="BG7" t="n">
@@ -3651,10 +3651,10 @@
         </is>
       </c>
       <c r="N8" t="n">
-        <v>50.70179748535156</v>
+        <v>50.7017974853516</v>
       </c>
       <c r="O8" t="n">
-        <v>-3.534698486328125</v>
+        <v>-3.53469848632812</v>
       </c>
       <c r="P8" t="inlineStr">
         <is>
@@ -3738,7 +3738,7 @@
       </c>
       <c r="BE8" t="inlineStr">
         <is>
-          <t>offer at least one portion of fresh fruit and vegetables everyday,are void of trans-fats* (artificially created fats used in the manufacture of foods to increase shelf life and the flavour-stability of foods. They are also often found in fast food, margarine, cakes and biscuits),offer added-sugar free days,offer mainly wholemeal carbohydrates (whole-grain bread, brown rice, or pasta for example),offer only high quality grass-fed meat options,Other, please specify below:</t>
+          <t>offer at least one portion of fresh fruit and vegetables everyday,are void of trans-fats* (artificially created fats used in the manufacture of foods to increase shelf life and the flavour-stability of foods. They are also often found in fast food; margarine; cakes and biscuits),offer added-sugar free days,offer mainly wholemeal carbohydrates (whole-grain bread; brown rice; or pasta for example),offer only high quality grass-fed meat options,Other, please specify below:</t>
         </is>
       </c>
       <c r="BF8" t="inlineStr">
@@ -3751,7 +3751,7 @@
       </c>
       <c r="BH8" t="inlineStr">
         <is>
-          <t>reduce high-carbon &amp; water footprint foods (meat and dairy, for example),minimise waste,contain locally sourced ingredients,contain organically sourced ingredients,contain  seasonally sourced ingredients,are cooked from scratch in the school kitchen,meet all dietary requirements,should be enjoyed by pupils,offer high quality grass-fed meat options,Other, please specify below:</t>
+          <t>reduce high-carbon &amp; water footprint foods (meat and dairy; for example),minimise waste,contain locally sourced ingredients,contain organically sourced ingredients,contain  seasonally sourced ingredients,are cooked from scratch in the school kitchen,meet all dietary requirements,should be enjoyed by pupils,offer high quality grass-fed meat options,Other, please specify below:</t>
         </is>
       </c>
       <c r="BI8" t="inlineStr">
@@ -4018,7 +4018,7 @@
         <v>51.068603515625</v>
       </c>
       <c r="O9" t="n">
-        <v>-4.020294189453125</v>
+        <v>-4.02029418945313</v>
       </c>
       <c r="P9" t="inlineStr">
         <is>
@@ -4228,10 +4228,10 @@
         </is>
       </c>
       <c r="N10" t="n">
-        <v>50.70179748535156</v>
+        <v>50.7017974853516</v>
       </c>
       <c r="O10" t="n">
-        <v>-3.534698486328125</v>
+        <v>-3.53469848632812</v>
       </c>
       <c r="P10" t="inlineStr">
         <is>
@@ -4320,7 +4320,7 @@
       </c>
       <c r="BE10" t="inlineStr">
         <is>
-          <t>offer at least one portion of fresh fruit and vegetables everyday,offer added-sugar free days,offer mainly wholemeal carbohydrates (whole-grain bread, brown rice, or pasta for example)</t>
+          <t>offer at least one portion of fresh fruit and vegetables everyday,offer added-sugar free days,offer mainly wholemeal carbohydrates (whole-grain bread; brown rice; or pasta for example)</t>
         </is>
       </c>
       <c r="BG10" t="n">
@@ -4328,7 +4328,7 @@
       </c>
       <c r="BH10" t="inlineStr">
         <is>
-          <t>reduce high-carbon &amp; water footprint foods (meat and dairy, for example),minimise waste,contain locally sourced ingredients,contain organically sourced ingredients,contain  seasonally sourced ingredients,are cooked from scratch in the school kitchen,meet all dietary requirements,should be enjoyed by pupils,offer high quality grass-fed meat options</t>
+          <t>reduce high-carbon &amp; water footprint foods (meat and dairy; for example),minimise waste,contain locally sourced ingredients,contain organically sourced ingredients,contain  seasonally sourced ingredients,are cooked from scratch in the school kitchen,meet all dietary requirements,should be enjoyed by pupils,offer high quality grass-fed meat options</t>
         </is>
       </c>
       <c r="BJ10" t="n">
@@ -4456,10 +4456,10 @@
         </is>
       </c>
       <c r="N11" t="n">
-        <v>50.38810729980469</v>
+        <v>50.3881072998047</v>
       </c>
       <c r="O11" t="n">
-        <v>-4.132400512695312</v>
+        <v>-4.13240051269531</v>
       </c>
       <c r="P11" t="inlineStr">
         <is>
@@ -4528,7 +4528,7 @@
       </c>
       <c r="BE11" t="inlineStr">
         <is>
-          <t>offer at least one portion of fresh fruit and vegetables everyday,offer mainly wholemeal carbohydrates (whole-grain bread, brown rice, or pasta for example),offer only high quality grass-fed meat options</t>
+          <t>offer at least one portion of fresh fruit and vegetables everyday,offer mainly wholemeal carbohydrates (whole-grain bread; brown rice; or pasta for example),offer only high quality grass-fed meat options</t>
         </is>
       </c>
       <c r="BG11" t="n">
@@ -4536,7 +4536,7 @@
       </c>
       <c r="BH11" t="inlineStr">
         <is>
-          <t>reduce high-carbon &amp; water footprint foods (meat and dairy, for example),minimise waste,contain locally sourced ingredients,contain  seasonally sourced ingredients,are cooked from scratch in the school kitchen,should be enjoyed by pupils,offer high quality grass-fed meat options</t>
+          <t>reduce high-carbon &amp; water footprint foods (meat and dairy; for example),minimise waste,contain locally sourced ingredients,contain  seasonally sourced ingredients,are cooked from scratch in the school kitchen,should be enjoyed by pupils,offer high quality grass-fed meat options</t>
         </is>
       </c>
       <c r="BJ11" t="n">
@@ -4785,10 +4785,10 @@
         </is>
       </c>
       <c r="N12" t="n">
-        <v>52.00100708007812</v>
+        <v>52.0010070800781</v>
       </c>
       <c r="O12" t="n">
-        <v>-0.2270050048828125</v>
+        <v>-0.227005004882812</v>
       </c>
       <c r="P12" t="inlineStr">
         <is>
@@ -4857,7 +4857,7 @@
       </c>
       <c r="BE12" t="inlineStr">
         <is>
-          <t>offer at least one portion of fresh fruit and vegetables everyday,offer fruit only, or fruit-based puddings,offer mainly wholemeal carbohydrates (whole-grain bread, brown rice, or pasta for example)</t>
+          <t>offer at least one portion of fresh fruit and vegetables everyday,offer fruit only, or fruit-based puddings,offer mainly wholemeal carbohydrates (whole-grain bread; brown rice; or pasta for example)</t>
         </is>
       </c>
       <c r="BG12" t="n">
@@ -5149,10 +5149,10 @@
         </is>
       </c>
       <c r="N13" t="n">
-        <v>50.70179748535156</v>
+        <v>50.7017974853516</v>
       </c>
       <c r="O13" t="n">
-        <v>-3.534698486328125</v>
+        <v>-3.53469848632812</v>
       </c>
       <c r="P13" t="inlineStr">
         <is>
@@ -5231,7 +5231,7 @@
       </c>
       <c r="BE13" t="inlineStr">
         <is>
-          <t>offer at least one portion of fresh fruit and vegetables everyday,offer mainly wholemeal carbohydrates (whole-grain bread, brown rice, or pasta for example),offer only high quality grass-fed meat options</t>
+          <t>offer at least one portion of fresh fruit and vegetables everyday,offer mainly wholemeal carbohydrates (whole-grain bread; brown rice; or pasta for example),offer only high quality grass-fed meat options</t>
         </is>
       </c>
       <c r="BG13" t="n">
@@ -5239,7 +5239,7 @@
       </c>
       <c r="BH13" t="inlineStr">
         <is>
-          <t>reduce high-carbon &amp; water footprint foods (meat and dairy, for example),minimise waste,contain locally sourced ingredients,contain organically sourced ingredients,contain  seasonally sourced ingredients,meet all dietary requirements,should be enjoyed by pupils,offer high quality grass-fed meat options</t>
+          <t>reduce high-carbon &amp; water footprint foods (meat and dairy; for example),minimise waste,contain locally sourced ingredients,contain organically sourced ingredients,contain  seasonally sourced ingredients,meet all dietary requirements,should be enjoyed by pupils,offer high quality grass-fed meat options</t>
         </is>
       </c>
       <c r="BJ13" t="n">
@@ -5498,10 +5498,10 @@
         </is>
       </c>
       <c r="N14" t="n">
-        <v>50.47880554199219</v>
+        <v>50.4788055419922</v>
       </c>
       <c r="O14" t="n">
-        <v>-3.544601440429688</v>
+        <v>-3.54460144042969</v>
       </c>
       <c r="P14" t="inlineStr">
         <is>
@@ -5570,7 +5570,7 @@
       </c>
       <c r="BE14" t="inlineStr">
         <is>
-          <t>offer at least one portion of fresh fruit and vegetables everyday,are void of trans-fats* (artificially created fats used in the manufacture of foods to increase shelf life and the flavour-stability of foods. They are also often found in fast food, margarine, cakes and biscuits),offer only high quality grass-fed meat options</t>
+          <t>offer at least one portion of fresh fruit and vegetables everyday,are void of trans-fats* (artificially created fats used in the manufacture of foods to increase shelf life and the flavour-stability of foods. They are also often found in fast food; margarine; cakes and biscuits),offer only high quality grass-fed meat options</t>
         </is>
       </c>
       <c r="BG14" t="n">
@@ -5827,7 +5827,7 @@
         </is>
       </c>
       <c r="N15" t="n">
-        <v>51.49639892578125</v>
+        <v>51.4963989257813</v>
       </c>
       <c r="O15" t="n">
         <v>-0.122406005859375</v>
@@ -5907,7 +5907,7 @@
       </c>
       <c r="BH15" t="inlineStr">
         <is>
-          <t>reduce high-carbon &amp; water footprint foods (meat and dairy, for example),minimise waste,contain organically sourced ingredients,contain  seasonally sourced ingredients,meet all dietary requirements,should be enjoyed by pupils</t>
+          <t>reduce high-carbon &amp; water footprint foods (meat and dairy; for example),minimise waste,contain organically sourced ingredients,contain  seasonally sourced ingredients,meet all dietary requirements,should be enjoyed by pupils</t>
         </is>
       </c>
       <c r="BJ15" t="n">
@@ -6035,7 +6035,7 @@
         </is>
       </c>
       <c r="N16" t="n">
-        <v>51.49639892578125</v>
+        <v>51.4963989257813</v>
       </c>
       <c r="O16" t="n">
         <v>-0.122406005859375</v>
@@ -6243,10 +6243,10 @@
         </is>
       </c>
       <c r="N17" t="n">
-        <v>50.52589416503906</v>
+        <v>50.5258941650391</v>
       </c>
       <c r="O17" t="n">
-        <v>-3.616500854492188</v>
+        <v>-3.61650085449219</v>
       </c>
       <c r="P17" t="inlineStr">
         <is>
@@ -6315,7 +6315,7 @@
       </c>
       <c r="BE17" t="inlineStr">
         <is>
-          <t>offer at least one portion of fresh fruit and vegetables everyday,offer mainly wholemeal carbohydrates (whole-grain bread, brown rice, or pasta for example)</t>
+          <t>offer at least one portion of fresh fruit and vegetables everyday,offer mainly wholemeal carbohydrates (whole-grain bread; brown rice; or pasta for example)</t>
         </is>
       </c>
       <c r="BH17" t="inlineStr">
@@ -6594,7 +6594,7 @@
         <v>50.7449951171875</v>
       </c>
       <c r="O18" t="n">
-        <v>-1.852401733398438</v>
+        <v>-1.85240173339844</v>
       </c>
       <c r="P18" t="inlineStr">
         <is>
@@ -6658,7 +6658,7 @@
       </c>
       <c r="BE18" t="inlineStr">
         <is>
-          <t>offer at least one portion of fresh fruit and vegetables everyday,are void of trans-fats* (artificially created fats used in the manufacture of foods to increase shelf life and the flavour-stability of foods. They are also often found in fast food, margarine, cakes and biscuits),offer mainly wholemeal carbohydrates (whole-grain bread, brown rice, or pasta for example)</t>
+          <t>offer at least one portion of fresh fruit and vegetables everyday,are void of trans-fats* (artificially created fats used in the manufacture of foods to increase shelf life and the flavour-stability of foods. They are also often found in fast food; margarine; cakes and biscuits),offer mainly wholemeal carbohydrates (whole-grain bread; brown rice; or pasta for example)</t>
         </is>
       </c>
       <c r="BG18" t="n">
@@ -6666,7 +6666,7 @@
       </c>
       <c r="BH18" t="inlineStr">
         <is>
-          <t>reduce high-carbon &amp; water footprint foods (meat and dairy, for example),minimise waste,contain locally sourced ingredients,contain organically sourced ingredients,contain  seasonally sourced ingredients,are cooked from scratch in the school kitchen,should be enjoyed by pupils</t>
+          <t>reduce high-carbon &amp; water footprint foods (meat and dairy; for example),minimise waste,contain locally sourced ingredients,contain organically sourced ingredients,contain  seasonally sourced ingredients,are cooked from scratch in the school kitchen,should be enjoyed by pupils</t>
         </is>
       </c>
       <c r="BJ18" t="n">
@@ -6915,10 +6915,10 @@
         </is>
       </c>
       <c r="N19" t="n">
-        <v>50.70179748535156</v>
+        <v>50.7017974853516</v>
       </c>
       <c r="O19" t="n">
-        <v>-3.534698486328125</v>
+        <v>-3.53469848632812</v>
       </c>
       <c r="P19" t="inlineStr">
         <is>
@@ -7005,7 +7005,7 @@
       </c>
       <c r="BH19" t="inlineStr">
         <is>
-          <t>reduce high-carbon &amp; water footprint foods (meat and dairy, for example),contain locally sourced ingredients,should be enjoyed by pupils</t>
+          <t>reduce high-carbon &amp; water footprint foods (meat and dairy; for example),contain locally sourced ingredients,should be enjoyed by pupils</t>
         </is>
       </c>
       <c r="BJ19" t="n">
@@ -7254,10 +7254,10 @@
         </is>
       </c>
       <c r="N20" t="n">
-        <v>50.70179748535156</v>
+        <v>50.7017974853516</v>
       </c>
       <c r="O20" t="n">
-        <v>-3.534698486328125</v>
+        <v>-3.53469848632812</v>
       </c>
       <c r="P20" t="inlineStr">
         <is>
@@ -7336,7 +7336,7 @@
       </c>
       <c r="BE20" t="inlineStr">
         <is>
-          <t>offer at least one portion of fresh fruit and vegetables everyday,are void of trans-fats* (artificially created fats used in the manufacture of foods to increase shelf life and the flavour-stability of foods. They are also often found in fast food, margarine, cakes and biscuits),offer mainly wholemeal carbohydrates (whole-grain bread, brown rice, or pasta for example),offer only high quality grass-fed meat options</t>
+          <t>offer at least one portion of fresh fruit and vegetables everyday,are void of trans-fats* (artificially created fats used in the manufacture of foods to increase shelf life and the flavour-stability of foods. They are also often found in fast food; margarine; cakes and biscuits),offer mainly wholemeal carbohydrates (whole-grain bread; brown rice; or pasta for example),offer only high quality grass-fed meat options</t>
         </is>
       </c>
       <c r="BG20" t="n">
@@ -7344,7 +7344,7 @@
       </c>
       <c r="BH20" t="inlineStr">
         <is>
-          <t>reduce high-carbon &amp; water footprint foods (meat and dairy, for example),minimise waste,contain locally sourced ingredients,should be enjoyed by pupils</t>
+          <t>reduce high-carbon &amp; water footprint foods (meat and dairy; for example),minimise waste,contain locally sourced ingredients,should be enjoyed by pupils</t>
         </is>
       </c>
       <c r="BJ20" t="n">
@@ -7653,10 +7653,10 @@
         </is>
       </c>
       <c r="N21" t="n">
-        <v>50.70179748535156</v>
+        <v>50.7017974853516</v>
       </c>
       <c r="O21" t="n">
-        <v>-3.534698486328125</v>
+        <v>-3.53469848632812</v>
       </c>
       <c r="P21" t="inlineStr">
         <is>
@@ -7858,10 +7858,10 @@
         </is>
       </c>
       <c r="N22" t="n">
-        <v>50.73739624023438</v>
+        <v>50.7373962402344</v>
       </c>
       <c r="O22" t="n">
-        <v>-3.470794677734375</v>
+        <v>-3.47079467773437</v>
       </c>
       <c r="P22" t="inlineStr">
         <is>
@@ -7915,7 +7915,7 @@
       </c>
       <c r="BE22" t="inlineStr">
         <is>
-          <t>are void of trans-fats* (artificially created fats used in the manufacture of foods to increase shelf life and the flavour-stability of foods. They are also often found in fast food, margarine, cakes and biscuits)</t>
+          <t>are void of trans-fats* (artificially created fats used in the manufacture of foods to increase shelf life and the flavour-stability of foods. They are also often found in fast food; margarine; cakes and biscuits)</t>
         </is>
       </c>
       <c r="BG22" t="n">
@@ -8059,7 +8059,7 @@
         <v>51.2279052734375</v>
       </c>
       <c r="O23" t="n">
-        <v>-2.526092529296875</v>
+        <v>-2.52609252929687</v>
       </c>
       <c r="P23" t="inlineStr">
         <is>
@@ -8143,7 +8143,7 @@
       </c>
       <c r="BE23" t="inlineStr">
         <is>
-          <t>offer at least one portion of fresh fruit and vegetables everyday,offer mainly wholemeal carbohydrates (whole-grain bread, brown rice, or pasta for example)</t>
+          <t>offer at least one portion of fresh fruit and vegetables everyday,offer mainly wholemeal carbohydrates (whole-grain bread; brown rice; or pasta for example)</t>
         </is>
       </c>
       <c r="BG23" t="n">
@@ -8289,10 +8289,10 @@
         </is>
       </c>
       <c r="N24" t="n">
-        <v>50.73739624023438</v>
+        <v>50.7373962402344</v>
       </c>
       <c r="O24" t="n">
-        <v>-3.470794677734375</v>
+        <v>-3.47079467773437</v>
       </c>
       <c r="P24" t="inlineStr">
         <is>
@@ -8379,7 +8379,7 @@
       </c>
       <c r="BH24" t="inlineStr">
         <is>
-          <t>reduce high-carbon &amp; water footprint foods (meat and dairy, for example),minimise waste,contain locally sourced ingredients</t>
+          <t>reduce high-carbon &amp; water footprint foods (meat and dairy; for example),minimise waste,contain locally sourced ingredients</t>
         </is>
       </c>
       <c r="BJ24" t="n">
@@ -8507,10 +8507,10 @@
         </is>
       </c>
       <c r="N25" t="n">
-        <v>50.38810729980469</v>
+        <v>50.3881072998047</v>
       </c>
       <c r="O25" t="n">
-        <v>-4.132400512695312</v>
+        <v>-4.13240051269531</v>
       </c>
       <c r="P25" t="inlineStr">
         <is>
@@ -8594,7 +8594,7 @@
       </c>
       <c r="BE25" t="inlineStr">
         <is>
-          <t>offer at least one portion of fresh fruit and vegetables everyday,are void of trans-fats* (artificially created fats used in the manufacture of foods to increase shelf life and the flavour-stability of foods. They are also often found in fast food, margarine, cakes and biscuits),offer only high quality grass-fed meat options</t>
+          <t>offer at least one portion of fresh fruit and vegetables everyday,are void of trans-fats* (artificially created fats used in the manufacture of foods to increase shelf life and the flavour-stability of foods. They are also often found in fast food; margarine; cakes and biscuits),offer only high quality grass-fed meat options</t>
         </is>
       </c>
       <c r="BG25" t="n">
@@ -8730,10 +8730,10 @@
         </is>
       </c>
       <c r="N26" t="n">
-        <v>50.73210144042969</v>
+        <v>50.7321014404297</v>
       </c>
       <c r="O26" t="n">
-        <v>-3.529998779296875</v>
+        <v>-3.52999877929687</v>
       </c>
       <c r="P26" t="inlineStr">
         <is>
@@ -8797,7 +8797,7 @@
       </c>
       <c r="BE26" t="inlineStr">
         <is>
-          <t>offer at least one portion of fresh fruit and vegetables everyday,are void of trans-fats* (artificially created fats used in the manufacture of foods to increase shelf life and the flavour-stability of foods. They are also often found in fast food, margarine, cakes and biscuits),offer mainly wholemeal carbohydrates (whole-grain bread, brown rice, or pasta for example),offer only high quality grass-fed meat options</t>
+          <t>offer at least one portion of fresh fruit and vegetables everyday,are void of trans-fats* (artificially created fats used in the manufacture of foods to increase shelf life and the flavour-stability of foods. They are also often found in fast food; margarine; cakes and biscuits),offer mainly wholemeal carbohydrates (whole-grain bread; brown rice; or pasta for example),offer only high quality grass-fed meat options</t>
         </is>
       </c>
       <c r="BG26" t="n">
@@ -8805,7 +8805,7 @@
       </c>
       <c r="BH26" t="inlineStr">
         <is>
-          <t>reduce high-carbon &amp; water footprint foods (meat and dairy, for example),minimise waste,contain locally sourced ingredients,contain organically sourced ingredients,contain  seasonally sourced ingredients,are cooked from scratch in the school kitchen,meet all dietary requirements,should be enjoyed by pupils,offer high quality grass-fed meat options</t>
+          <t>reduce high-carbon &amp; water footprint foods (meat and dairy; for example),minimise waste,contain locally sourced ingredients,contain organically sourced ingredients,contain  seasonally sourced ingredients,are cooked from scratch in the school kitchen,meet all dietary requirements,should be enjoyed by pupils,offer high quality grass-fed meat options</t>
         </is>
       </c>
       <c r="BJ26" t="n">
@@ -9049,7 +9049,7 @@
         </is>
       </c>
       <c r="N27" t="n">
-        <v>51.64840698242188</v>
+        <v>51.6484069824219</v>
       </c>
       <c r="O27" t="n">
         <v>-0.49310302734375</v>
@@ -9129,7 +9129,7 @@
       </c>
       <c r="BH27" t="inlineStr">
         <is>
-          <t>reduce high-carbon &amp; water footprint foods (meat and dairy, for example),minimise waste,should be enjoyed by pupils</t>
+          <t>reduce high-carbon &amp; water footprint foods (meat and dairy; for example),minimise waste,should be enjoyed by pupils</t>
         </is>
       </c>
       <c r="BJ27" t="n">
@@ -9247,10 +9247,10 @@
         </is>
       </c>
       <c r="N28" t="n">
-        <v>50.43809509277344</v>
+        <v>50.4380950927734</v>
       </c>
       <c r="O28" t="n">
-        <v>-4.082992553710938</v>
+        <v>-4.08299255371094</v>
       </c>
       <c r="P28" t="inlineStr">
         <is>
@@ -9310,10 +9310,10 @@
         </is>
       </c>
       <c r="N29" t="n">
-        <v>50.73210144042969</v>
+        <v>50.7321014404297</v>
       </c>
       <c r="O29" t="n">
-        <v>-3.529998779296875</v>
+        <v>-3.52999877929687</v>
       </c>
       <c r="P29" t="inlineStr">
         <is>
@@ -9382,7 +9382,7 @@
       </c>
       <c r="BE29" t="inlineStr">
         <is>
-          <t>offer at least one portion of fresh fruit and vegetables everyday,offer mainly wholemeal carbohydrates (whole-grain bread, brown rice, or pasta for example),offer only high quality grass-fed meat options</t>
+          <t>offer at least one portion of fresh fruit and vegetables everyday,offer mainly wholemeal carbohydrates (whole-grain bread; brown rice; or pasta for example),offer only high quality grass-fed meat options</t>
         </is>
       </c>
       <c r="BG29" t="n">
@@ -9634,10 +9634,10 @@
         </is>
       </c>
       <c r="N30" t="n">
-        <v>50.70179748535156</v>
+        <v>50.7017974853516</v>
       </c>
       <c r="O30" t="n">
-        <v>-3.534698486328125</v>
+        <v>-3.53469848632812</v>
       </c>
       <c r="P30" t="inlineStr">
         <is>
@@ -9697,10 +9697,10 @@
         </is>
       </c>
       <c r="N31" t="n">
-        <v>50.70179748535156</v>
+        <v>50.7017974853516</v>
       </c>
       <c r="O31" t="n">
-        <v>-3.534698486328125</v>
+        <v>-3.53469848632812</v>
       </c>
       <c r="P31" t="inlineStr">
         <is>
@@ -9764,7 +9764,7 @@
       </c>
       <c r="BE31" t="inlineStr">
         <is>
-          <t>offer at least one portion of fresh fruit and vegetables everyday,are void of trans-fats* (artificially created fats used in the manufacture of foods to increase shelf life and the flavour-stability of foods. They are also often found in fast food, margarine, cakes and biscuits),offer mainly wholemeal carbohydrates (whole-grain bread, brown rice, or pasta for example),offer only high quality grass-fed meat options</t>
+          <t>offer at least one portion of fresh fruit and vegetables everyday,are void of trans-fats* (artificially created fats used in the manufacture of foods to increase shelf life and the flavour-stability of foods. They are also often found in fast food; margarine; cakes and biscuits),offer mainly wholemeal carbohydrates (whole-grain bread; brown rice; or pasta for example),offer only high quality grass-fed meat options</t>
         </is>
       </c>
       <c r="BG31" t="n">
@@ -10190,10 +10190,10 @@
         </is>
       </c>
       <c r="N33" t="n">
-        <v>52.14570617675781</v>
+        <v>52.1457061767578</v>
       </c>
       <c r="O33" t="n">
-        <v>-0.8802947998046875</v>
+        <v>-0.8802947998046881</v>
       </c>
       <c r="P33" t="inlineStr">
         <is>
@@ -10665,7 +10665,7 @@
       </c>
       <c r="BE36" t="inlineStr">
         <is>
-          <t>offer at least one portion of fresh fruit and vegetables everyday,are void of trans-fats* (artificially created fats used in the manufacture of foods to increase shelf life and the flavour-stability of foods. They are also often found in fast food, margarine, cakes and biscuits),offer added-sugar free days,offer mainly wholemeal carbohydrates (whole-grain bread, brown rice, or pasta for example)</t>
+          <t>offer at least one portion of fresh fruit and vegetables everyday,are void of trans-fats* (artificially created fats used in the manufacture of foods to increase shelf life and the flavour-stability of foods. They are also often found in fast food; margarine; cakes and biscuits),offer added-sugar free days,offer mainly wholemeal carbohydrates (whole-grain bread; brown rice; or pasta for example)</t>
         </is>
       </c>
       <c r="BG36" t="n">
@@ -10673,7 +10673,7 @@
       </c>
       <c r="BH36" t="inlineStr">
         <is>
-          <t>reduce high-carbon &amp; water footprint foods (meat and dairy, for example),minimise waste,contain locally sourced ingredients,contain organically sourced ingredients,contain  seasonally sourced ingredients,are cooked from scratch in the school kitchen</t>
+          <t>reduce high-carbon &amp; water footprint foods (meat and dairy; for example),minimise waste,contain locally sourced ingredients,contain organically sourced ingredients,contain  seasonally sourced ingredients,are cooked from scratch in the school kitchen</t>
         </is>
       </c>
       <c r="BJ36" t="n">
@@ -10973,7 +10973,7 @@
       </c>
       <c r="BE37" t="inlineStr">
         <is>
-          <t>offer at least one portion of fresh fruit and vegetables everyday,offer fruit only, or fruit-based puddings,are void of trans-fats* (artificially created fats used in the manufacture of foods to increase shelf life and the flavour-stability of foods. They are also often found in fast food, margarine, cakes and biscuits),offer added-sugar free days,offer mainly wholemeal carbohydrates (whole-grain bread, brown rice, or pasta for example),offer only high quality grass-fed meat options</t>
+          <t>offer at least one portion of fresh fruit and vegetables everyday,offer fruit only, or fruit-based puddings,are void of trans-fats* (artificially created fats used in the manufacture of foods to increase shelf life and the flavour-stability of foods. They are also often found in fast food; margarine; cakes and biscuits),offer added-sugar free days,offer mainly wholemeal carbohydrates (whole-grain bread; brown rice; or pasta for example),offer only high quality grass-fed meat options</t>
         </is>
       </c>
       <c r="BG37" t="n">
@@ -10981,7 +10981,7 @@
       </c>
       <c r="BH37" t="inlineStr">
         <is>
-          <t>reduce high-carbon &amp; water footprint foods (meat and dairy, for example),minimise waste,contain locally sourced ingredients,contain organically sourced ingredients,contain  seasonally sourced ingredients,are cooked from scratch in the school kitchen,meet all dietary requirements,should be enjoyed by pupils,offer high quality grass-fed meat options</t>
+          <t>reduce high-carbon &amp; water footprint foods (meat and dairy; for example),minimise waste,contain locally sourced ingredients,contain organically sourced ingredients,contain  seasonally sourced ingredients,are cooked from scratch in the school kitchen,meet all dietary requirements,should be enjoyed by pupils,offer high quality grass-fed meat options</t>
         </is>
       </c>
       <c r="BJ37" t="n">
@@ -11581,7 +11581,7 @@
       </c>
       <c r="BE40" t="inlineStr">
         <is>
-          <t>offer at least one portion of fresh fruit and vegetables everyday,offer fruit only, or fruit-based puddings,are void of trans-fats* (artificially created fats used in the manufacture of foods to increase shelf life and the flavour-stability of foods. They are also often found in fast food, margarine, cakes and biscuits),offer mainly wholemeal carbohydrates (whole-grain bread, brown rice, or pasta for example),offer only high quality grass-fed meat options,Other, please specify below:</t>
+          <t>offer at least one portion of fresh fruit and vegetables everyday,offer fruit only, or fruit-based puddings,are void of trans-fats* (artificially created fats used in the manufacture of foods to increase shelf life and the flavour-stability of foods. They are also often found in fast food; margarine; cakes and biscuits),offer mainly wholemeal carbohydrates (whole-grain bread; brown rice; or pasta for example),offer only high quality grass-fed meat options,Other, please specify below:</t>
         </is>
       </c>
       <c r="BF40" t="inlineStr">
@@ -11594,7 +11594,7 @@
       </c>
       <c r="BH40" t="inlineStr">
         <is>
-          <t>reduce high-carbon &amp; water footprint foods (meat and dairy, for example),minimise waste,contain locally sourced ingredients,contain organically sourced ingredients,contain  seasonally sourced ingredients,are cooked from scratch in the school kitchen,meet all dietary requirements,should be enjoyed by pupils,offer high quality grass-fed meat options</t>
+          <t>reduce high-carbon &amp; water footprint foods (meat and dairy; for example),minimise waste,contain locally sourced ingredients,contain organically sourced ingredients,contain  seasonally sourced ingredients,are cooked from scratch in the school kitchen,meet all dietary requirements,should be enjoyed by pupils,offer high quality grass-fed meat options</t>
         </is>
       </c>
       <c r="BJ40" t="n">
@@ -11933,7 +11933,7 @@
       </c>
       <c r="BH42" t="inlineStr">
         <is>
-          <t>reduce high-carbon &amp; water footprint foods (meat and dairy, for example),minimise waste,contain locally sourced ingredients,contain organically sourced ingredients,contain  seasonally sourced ingredients,are cooked from scratch in the school kitchen,meet all dietary requirements,should be enjoyed by pupils,offer high quality grass-fed meat options</t>
+          <t>reduce high-carbon &amp; water footprint foods (meat and dairy; for example),minimise waste,contain locally sourced ingredients,contain organically sourced ingredients,contain  seasonally sourced ingredients,are cooked from scratch in the school kitchen,meet all dietary requirements,should be enjoyed by pupils,offer high quality grass-fed meat options</t>
         </is>
       </c>
       <c r="BJ42" t="n">
@@ -12202,7 +12202,7 @@
       </c>
       <c r="BE43" t="inlineStr">
         <is>
-          <t>offer at least one portion of fresh fruit and vegetables everyday,offer mainly wholemeal carbohydrates (whole-grain bread, brown rice, or pasta for example)</t>
+          <t>offer at least one portion of fresh fruit and vegetables everyday,offer mainly wholemeal carbohydrates (whole-grain bread; brown rice; or pasta for example)</t>
         </is>
       </c>
       <c r="BG43" t="n">
@@ -12210,7 +12210,7 @@
       </c>
       <c r="BH43" t="inlineStr">
         <is>
-          <t>reduce high-carbon &amp; water footprint foods (meat and dairy, for example),minimise waste,contain locally sourced ingredients,contain  seasonally sourced ingredients</t>
+          <t>reduce high-carbon &amp; water footprint foods (meat and dairy; for example),minimise waste,contain locally sourced ingredients,contain  seasonally sourced ingredients</t>
         </is>
       </c>
       <c r="BJ43" t="n">
@@ -12413,10 +12413,10 @@
         </is>
       </c>
       <c r="N44" t="n">
-        <v>50.73739624023438</v>
+        <v>50.7373962402344</v>
       </c>
       <c r="O44" t="n">
-        <v>-3.470794677734375</v>
+        <v>-3.47079467773437</v>
       </c>
       <c r="P44" t="inlineStr">
         <is>
@@ -12505,7 +12505,7 @@
       </c>
       <c r="BE44" t="inlineStr">
         <is>
-          <t>offer at least one portion of fresh fruit and vegetables everyday,are void of trans-fats* (artificially created fats used in the manufacture of foods to increase shelf life and the flavour-stability of foods. They are also often found in fast food, margarine, cakes and biscuits),offer mainly wholemeal carbohydrates (whole-grain bread, brown rice, or pasta for example)</t>
+          <t>offer at least one portion of fresh fruit and vegetables everyday,are void of trans-fats* (artificially created fats used in the manufacture of foods to increase shelf life and the flavour-stability of foods. They are also often found in fast food; margarine; cakes and biscuits),offer mainly wholemeal carbohydrates (whole-grain bread; brown rice; or pasta for example)</t>
         </is>
       </c>
       <c r="BG44" t="n">
@@ -13021,7 +13021,7 @@
       </c>
       <c r="BE46" t="inlineStr">
         <is>
-          <t>offer at least one portion of fresh fruit and vegetables everyday,are void of trans-fats* (artificially created fats used in the manufacture of foods to increase shelf life and the flavour-stability of foods. They are also often found in fast food, margarine, cakes and biscuits),offer mainly wholemeal carbohydrates (whole-grain bread, brown rice, or pasta for example),offer only high quality grass-fed meat options</t>
+          <t>offer at least one portion of fresh fruit and vegetables everyday,are void of trans-fats* (artificially created fats used in the manufacture of foods to increase shelf life and the flavour-stability of foods. They are also often found in fast food; margarine; cakes and biscuits),offer mainly wholemeal carbohydrates (whole-grain bread; brown rice; or pasta for example),offer only high quality grass-fed meat options</t>
         </is>
       </c>
       <c r="BG46" t="n">
@@ -13029,7 +13029,7 @@
       </c>
       <c r="BH46" t="inlineStr">
         <is>
-          <t>reduce high-carbon &amp; water footprint foods (meat and dairy, for example),minimise waste,contain locally sourced ingredients,contain  seasonally sourced ingredients,are cooked from scratch in the school kitchen,meet all dietary requirements,should be enjoyed by pupils,offer high quality grass-fed meat options</t>
+          <t>reduce high-carbon &amp; water footprint foods (meat and dairy; for example),minimise waste,contain locally sourced ingredients,contain  seasonally sourced ingredients,are cooked from scratch in the school kitchen,meet all dietary requirements,should be enjoyed by pupils,offer high quality grass-fed meat options</t>
         </is>
       </c>
       <c r="BJ46" t="n">
@@ -13406,7 +13406,7 @@
       </c>
       <c r="BE48" t="inlineStr">
         <is>
-          <t>offer at least one portion of fresh fruit and vegetables everyday,are void of trans-fats* (artificially created fats used in the manufacture of foods to increase shelf life and the flavour-stability of foods. They are also often found in fast food, margarine, cakes and biscuits),offer mainly wholemeal carbohydrates (whole-grain bread, brown rice, or pasta for example),offer only high quality grass-fed meat options</t>
+          <t>offer at least one portion of fresh fruit and vegetables everyday,are void of trans-fats* (artificially created fats used in the manufacture of foods to increase shelf life and the flavour-stability of foods. They are also often found in fast food; margarine; cakes and biscuits),offer mainly wholemeal carbohydrates (whole-grain bread; brown rice; or pasta for example),offer only high quality grass-fed meat options</t>
         </is>
       </c>
       <c r="BG48" t="n">
@@ -13534,7 +13534,7 @@
       </c>
       <c r="BE49" t="inlineStr">
         <is>
-          <t>offer at least one portion of fresh fruit and vegetables everyday,are void of trans-fats* (artificially created fats used in the manufacture of foods to increase shelf life and the flavour-stability of foods. They are also often found in fast food, margarine, cakes and biscuits),offer mainly wholemeal carbohydrates (whole-grain bread, brown rice, or pasta for example),offer only high quality grass-fed meat options</t>
+          <t>offer at least one portion of fresh fruit and vegetables everyday,are void of trans-fats* (artificially created fats used in the manufacture of foods to increase shelf life and the flavour-stability of foods. They are also often found in fast food; margarine; cakes and biscuits),offer mainly wholemeal carbohydrates (whole-grain bread; brown rice; or pasta for example),offer only high quality grass-fed meat options</t>
         </is>
       </c>
       <c r="BG49" t="n">
@@ -13542,7 +13542,7 @@
       </c>
       <c r="BH49" t="inlineStr">
         <is>
-          <t>reduce high-carbon &amp; water footprint foods (meat and dairy, for example),minimise waste,contain locally sourced ingredients,contain organically sourced ingredients,contain  seasonally sourced ingredients,are cooked from scratch in the school kitchen,meet all dietary requirements,should be enjoyed by pupils,offer high quality grass-fed meat options</t>
+          <t>reduce high-carbon &amp; water footprint foods (meat and dairy; for example),minimise waste,contain locally sourced ingredients,contain organically sourced ingredients,contain  seasonally sourced ingredients,are cooked from scratch in the school kitchen,meet all dietary requirements,should be enjoyed by pupils,offer high quality grass-fed meat options</t>
         </is>
       </c>
       <c r="BJ49" t="n">
@@ -13670,10 +13670,10 @@
         </is>
       </c>
       <c r="N50" t="n">
-        <v>50.47799682617188</v>
+        <v>50.4779968261719</v>
       </c>
       <c r="O50" t="n">
-        <v>-3.518203735351562</v>
+        <v>-3.51820373535156</v>
       </c>
       <c r="P50" t="inlineStr">
         <is>
@@ -13999,10 +13999,10 @@
         </is>
       </c>
       <c r="N51" t="n">
-        <v>50.70179748535156</v>
+        <v>50.7017974853516</v>
       </c>
       <c r="O51" t="n">
-        <v>-3.534698486328125</v>
+        <v>-3.53469848632812</v>
       </c>
       <c r="P51" t="inlineStr">
         <is>
@@ -14081,7 +14081,7 @@
       </c>
       <c r="BE51" t="inlineStr">
         <is>
-          <t>offer at least one portion of fresh fruit and vegetables everyday,offer fruit only, or fruit-based puddings,offer added-sugar free days,offer mainly wholemeal carbohydrates (whole-grain bread, brown rice, or pasta for example),offer only high quality grass-fed meat options</t>
+          <t>offer at least one portion of fresh fruit and vegetables everyday,offer fruit only, or fruit-based puddings,offer added-sugar free days,offer mainly wholemeal carbohydrates (whole-grain bread; brown rice; or pasta for example),offer only high quality grass-fed meat options</t>
         </is>
       </c>
       <c r="BG51" t="n">
@@ -14089,7 +14089,7 @@
       </c>
       <c r="BH51" t="inlineStr">
         <is>
-          <t>reduce high-carbon &amp; water footprint foods (meat and dairy, for example),minimise waste,contain locally sourced ingredients,contain  seasonally sourced ingredients,are cooked from scratch in the school kitchen,meet all dietary requirements,should be enjoyed by pupils</t>
+          <t>reduce high-carbon &amp; water footprint foods (meat and dairy; for example),minimise waste,contain locally sourced ingredients,contain  seasonally sourced ingredients,are cooked from scratch in the school kitchen,meet all dietary requirements,should be enjoyed by pupils</t>
         </is>
       </c>
       <c r="BJ51" t="n">
@@ -14329,10 +14329,10 @@
         </is>
       </c>
       <c r="N53" t="n">
-        <v>50.73739624023438</v>
+        <v>50.7373962402344</v>
       </c>
       <c r="O53" t="n">
-        <v>-3.470794677734375</v>
+        <v>-3.47079467773437</v>
       </c>
       <c r="P53" t="inlineStr">
         <is>
@@ -14421,7 +14421,7 @@
       </c>
       <c r="BE53" t="inlineStr">
         <is>
-          <t>offer at least one portion of fresh fruit and vegetables everyday,are void of trans-fats* (artificially created fats used in the manufacture of foods to increase shelf life and the flavour-stability of foods. They are also often found in fast food, margarine, cakes and biscuits),offer added-sugar free days,offer mainly wholemeal carbohydrates (whole-grain bread, brown rice, or pasta for example)</t>
+          <t>offer at least one portion of fresh fruit and vegetables everyday,are void of trans-fats* (artificially created fats used in the manufacture of foods to increase shelf life and the flavour-stability of foods. They are also often found in fast food; margarine; cakes and biscuits),offer added-sugar free days,offer mainly wholemeal carbohydrates (whole-grain bread; brown rice; or pasta for example)</t>
         </is>
       </c>
       <c r="BG53" t="n">
@@ -14562,10 +14562,10 @@
         </is>
       </c>
       <c r="N54" t="n">
-        <v>51.43510437011719</v>
+        <v>51.4351043701172</v>
       </c>
       <c r="O54" t="n">
-        <v>-2.541900634765625</v>
+        <v>-2.54190063476562</v>
       </c>
       <c r="P54" t="inlineStr">
         <is>
@@ -14644,7 +14644,7 @@
       </c>
       <c r="BH54" t="inlineStr">
         <is>
-          <t>reduce high-carbon &amp; water footprint foods (meat and dairy, for example),minimise waste,contain locally sourced ingredients,contain  seasonally sourced ingredients,should be enjoyed by pupils</t>
+          <t>reduce high-carbon &amp; water footprint foods (meat and dairy; for example),minimise waste,contain locally sourced ingredients,contain  seasonally sourced ingredients,should be enjoyed by pupils</t>
         </is>
       </c>
       <c r="BK54" t="inlineStr">
@@ -14890,10 +14890,10 @@
         </is>
       </c>
       <c r="N55" t="n">
-        <v>50.70179748535156</v>
+        <v>50.7017974853516</v>
       </c>
       <c r="O55" t="n">
-        <v>-3.534698486328125</v>
+        <v>-3.53469848632812</v>
       </c>
       <c r="P55" t="inlineStr">
         <is>
@@ -15103,10 +15103,10 @@
         </is>
       </c>
       <c r="N56" t="n">
-        <v>50.47799682617188</v>
+        <v>50.4779968261719</v>
       </c>
       <c r="O56" t="n">
-        <v>-3.518203735351562</v>
+        <v>-3.51820373535156</v>
       </c>
       <c r="P56" t="inlineStr">
         <is>
@@ -15324,7 +15324,7 @@
         <v>50.5458984375</v>
       </c>
       <c r="O57" t="n">
-        <v>-3.534500122070312</v>
+        <v>-3.53450012207031</v>
       </c>
       <c r="P57" t="inlineStr">
         <is>
@@ -15408,7 +15408,7 @@
       </c>
       <c r="BE57" t="inlineStr">
         <is>
-          <t>offer at least one portion of fresh fruit and vegetables everyday,are void of trans-fats* (artificially created fats used in the manufacture of foods to increase shelf life and the flavour-stability of foods. They are also often found in fast food, margarine, cakes and biscuits),offer added-sugar free days</t>
+          <t>offer at least one portion of fresh fruit and vegetables everyday,are void of trans-fats* (artificially created fats used in the manufacture of foods to increase shelf life and the flavour-stability of foods. They are also often found in fast food; margarine; cakes and biscuits),offer added-sugar free days</t>
         </is>
       </c>
       <c r="BG57" t="n">
@@ -15416,7 +15416,7 @@
       </c>
       <c r="BH57" t="inlineStr">
         <is>
-          <t>reduce high-carbon &amp; water footprint foods (meat and dairy, for example),minimise waste,contain locally sourced ingredients,contain  seasonally sourced ingredients,should be enjoyed by pupils</t>
+          <t>reduce high-carbon &amp; water footprint foods (meat and dairy; for example),minimise waste,contain locally sourced ingredients,contain  seasonally sourced ingredients,should be enjoyed by pupils</t>
         </is>
       </c>
       <c r="BJ57" t="n">
@@ -15645,10 +15645,10 @@
         </is>
       </c>
       <c r="N58" t="n">
-        <v>50.39889526367188</v>
+        <v>50.3988952636719</v>
       </c>
       <c r="O58" t="n">
-        <v>-4.172698974609375</v>
+        <v>-4.17269897460938</v>
       </c>
       <c r="P58" t="inlineStr">
         <is>
@@ -15732,7 +15732,7 @@
       </c>
       <c r="BE58" t="inlineStr">
         <is>
-          <t>offer at least one portion of fresh fruit and vegetables everyday,are void of trans-fats* (artificially created fats used in the manufacture of foods to increase shelf life and the flavour-stability of foods. They are also often found in fast food, margarine, cakes and biscuits),offer added-sugar free days</t>
+          <t>offer at least one portion of fresh fruit and vegetables everyday,are void of trans-fats* (artificially created fats used in the manufacture of foods to increase shelf life and the flavour-stability of foods. They are also often found in fast food; margarine; cakes and biscuits),offer added-sugar free days</t>
         </is>
       </c>
       <c r="BG58" t="n">
@@ -15740,7 +15740,7 @@
       </c>
       <c r="BH58" t="inlineStr">
         <is>
-          <t>reduce high-carbon &amp; water footprint foods (meat and dairy, for example),minimise waste,contain locally sourced ingredients,contain  seasonally sourced ingredients,are cooked from scratch in the school kitchen,should be enjoyed by pupils</t>
+          <t>reduce high-carbon &amp; water footprint foods (meat and dairy; for example),minimise waste,contain locally sourced ingredients,contain  seasonally sourced ingredients,are cooked from scratch in the school kitchen,should be enjoyed by pupils</t>
         </is>
       </c>
       <c r="BJ58" t="n">
@@ -15994,10 +15994,10 @@
         </is>
       </c>
       <c r="N59" t="n">
-        <v>50.47880554199219</v>
+        <v>50.4788055419922</v>
       </c>
       <c r="O59" t="n">
-        <v>-3.544601440429688</v>
+        <v>-3.54460144042969</v>
       </c>
       <c r="P59" t="inlineStr">
         <is>
@@ -16094,7 +16094,7 @@
       </c>
       <c r="BH59" t="inlineStr">
         <is>
-          <t>reduce high-carbon &amp; water footprint foods (meat and dairy, for example),minimise waste,contain locally sourced ingredients,contain  seasonally sourced ingredients,meet all dietary requirements,should be enjoyed by pupils</t>
+          <t>reduce high-carbon &amp; water footprint foods (meat and dairy; for example),minimise waste,contain locally sourced ingredients,contain  seasonally sourced ingredients,meet all dietary requirements,should be enjoyed by pupils</t>
         </is>
       </c>
       <c r="BJ59" t="n">
@@ -16363,10 +16363,10 @@
         </is>
       </c>
       <c r="N60" t="n">
-        <v>50.47799682617188</v>
+        <v>50.4779968261719</v>
       </c>
       <c r="O60" t="n">
-        <v>-3.518203735351562</v>
+        <v>-3.51820373535156</v>
       </c>
       <c r="P60" t="inlineStr">
         <is>
@@ -16445,7 +16445,7 @@
       </c>
       <c r="BE60" t="inlineStr">
         <is>
-          <t>offer at least one portion of fresh fruit and vegetables everyday,are void of trans-fats* (artificially created fats used in the manufacture of foods to increase shelf life and the flavour-stability of foods. They are also often found in fast food, margarine, cakes and biscuits),offer mainly wholemeal carbohydrates (whole-grain bread, brown rice, or pasta for example)</t>
+          <t>offer at least one portion of fresh fruit and vegetables everyday,are void of trans-fats* (artificially created fats used in the manufacture of foods to increase shelf life and the flavour-stability of foods. They are also often found in fast food; margarine; cakes and biscuits),offer mainly wholemeal carbohydrates (whole-grain bread; brown rice; or pasta for example)</t>
         </is>
       </c>
       <c r="BG60" t="n">
@@ -16712,10 +16712,10 @@
         </is>
       </c>
       <c r="N61" t="n">
-        <v>50.70179748535156</v>
+        <v>50.7017974853516</v>
       </c>
       <c r="O61" t="n">
-        <v>-3.534698486328125</v>
+        <v>-3.53469848632812</v>
       </c>
       <c r="P61" t="inlineStr">
         <is>
@@ -16794,7 +16794,7 @@
       </c>
       <c r="BE61" t="inlineStr">
         <is>
-          <t>offer at least one portion of fresh fruit and vegetables everyday,are void of trans-fats* (artificially created fats used in the manufacture of foods to increase shelf life and the flavour-stability of foods. They are also often found in fast food, margarine, cakes and biscuits),offer added-sugar free days,offer mainly wholemeal carbohydrates (whole-grain bread, brown rice, or pasta for example),offer only high quality grass-fed meat options</t>
+          <t>offer at least one portion of fresh fruit and vegetables everyday,are void of trans-fats* (artificially created fats used in the manufacture of foods to increase shelf life and the flavour-stability of foods. They are also often found in fast food; margarine; cakes and biscuits),offer added-sugar free days,offer mainly wholemeal carbohydrates (whole-grain bread; brown rice; or pasta for example),offer only high quality grass-fed meat options</t>
         </is>
       </c>
       <c r="BG61" t="n">
@@ -16935,10 +16935,10 @@
         </is>
       </c>
       <c r="N62" t="n">
-        <v>50.38810729980469</v>
+        <v>50.3881072998047</v>
       </c>
       <c r="O62" t="n">
-        <v>-4.132400512695312</v>
+        <v>-4.13240051269531</v>
       </c>
       <c r="P62" t="inlineStr">
         <is>
@@ -17015,7 +17015,7 @@
       </c>
       <c r="BH62" t="inlineStr">
         <is>
-          <t>reduce high-carbon &amp; water footprint foods (meat and dairy, for example),minimise waste,contain locally sourced ingredients,contain organically sourced ingredients,contain  seasonally sourced ingredients,are cooked from scratch in the school kitchen,meet all dietary requirements,should be enjoyed by pupils,offer high quality grass-fed meat options</t>
+          <t>reduce high-carbon &amp; water footprint foods (meat and dairy; for example),minimise waste,contain locally sourced ingredients,contain organically sourced ingredients,contain  seasonally sourced ingredients,are cooked from scratch in the school kitchen,meet all dietary requirements,should be enjoyed by pupils,offer high quality grass-fed meat options</t>
         </is>
       </c>
       <c r="BJ62" t="n">
@@ -17244,7 +17244,7 @@
         </is>
       </c>
       <c r="N63" t="n">
-        <v>51.49639892578125</v>
+        <v>51.4963989257813</v>
       </c>
       <c r="O63" t="n">
         <v>-0.122406005859375</v>
@@ -17324,7 +17324,7 @@
       </c>
       <c r="BH63" t="inlineStr">
         <is>
-          <t>reduce high-carbon &amp; water footprint foods (meat and dairy, for example),minimise waste</t>
+          <t>reduce high-carbon &amp; water footprint foods (meat and dairy; for example),minimise waste</t>
         </is>
       </c>
       <c r="BJ63" t="n">
@@ -17578,10 +17578,10 @@
         </is>
       </c>
       <c r="N64" t="n">
-        <v>50.70179748535156</v>
+        <v>50.7017974853516</v>
       </c>
       <c r="O64" t="n">
-        <v>-3.534698486328125</v>
+        <v>-3.53469848632812</v>
       </c>
       <c r="P64" t="inlineStr">
         <is>
@@ -17892,10 +17892,10 @@
         </is>
       </c>
       <c r="N65" t="n">
-        <v>50.36799621582031</v>
+        <v>50.3679962158203</v>
       </c>
       <c r="O65" t="n">
-        <v>-4.132904052734375</v>
+        <v>-4.13290405273438</v>
       </c>
       <c r="P65" t="inlineStr">
         <is>
@@ -17964,7 +17964,7 @@
       </c>
       <c r="BE65" t="inlineStr">
         <is>
-          <t>offer at least one portion of fresh fruit and vegetables everyday,offer fruit only, or fruit-based puddings,are void of trans-fats* (artificially created fats used in the manufacture of foods to increase shelf life and the flavour-stability of foods. They are also often found in fast food, margarine, cakes and biscuits),offer mainly wholemeal carbohydrates (whole-grain bread, brown rice, or pasta for example),offer only high quality grass-fed meat options,Other, please specify below:</t>
+          <t>offer at least one portion of fresh fruit and vegetables everyday,offer fruit only, or fruit-based puddings,are void of trans-fats* (artificially created fats used in the manufacture of foods to increase shelf life and the flavour-stability of foods. They are also often found in fast food; margarine; cakes and biscuits),offer mainly wholemeal carbohydrates (whole-grain bread; brown rice; or pasta for example),offer only high quality grass-fed meat options,Other, please specify below:</t>
         </is>
       </c>
       <c r="BF65" t="inlineStr">
@@ -17977,7 +17977,7 @@
       </c>
       <c r="BH65" t="inlineStr">
         <is>
-          <t>reduce high-carbon &amp; water footprint foods (meat and dairy, for example),minimise waste,contain locally sourced ingredients,contain organically sourced ingredients,contain  seasonally sourced ingredients,are cooked from scratch in the school kitchen,meet all dietary requirements,offer high quality grass-fed meat options,Other, please specify below:</t>
+          <t>reduce high-carbon &amp; water footprint foods (meat and dairy; for example),minimise waste,contain locally sourced ingredients,contain organically sourced ingredients,contain  seasonally sourced ingredients,are cooked from scratch in the school kitchen,meet all dietary requirements,offer high quality grass-fed meat options,Other, please specify below:</t>
         </is>
       </c>
       <c r="BI65" t="inlineStr">
@@ -18125,10 +18125,10 @@
         </is>
       </c>
       <c r="N66" t="n">
-        <v>50.70179748535156</v>
+        <v>50.7017974853516</v>
       </c>
       <c r="O66" t="n">
-        <v>-3.534698486328125</v>
+        <v>-3.53469848632812</v>
       </c>
       <c r="P66" t="inlineStr">
         <is>
@@ -18197,7 +18197,7 @@
       </c>
       <c r="BE66" t="inlineStr">
         <is>
-          <t>offer at least one portion of fresh fruit and vegetables everyday,are void of trans-fats* (artificially created fats used in the manufacture of foods to increase shelf life and the flavour-stability of foods. They are also often found in fast food, margarine, cakes and biscuits),offer mainly wholemeal carbohydrates (whole-grain bread, brown rice, or pasta for example),offer only high quality grass-fed meat options</t>
+          <t>offer at least one portion of fresh fruit and vegetables everyday,are void of trans-fats* (artificially created fats used in the manufacture of foods to increase shelf life and the flavour-stability of foods. They are also often found in fast food; margarine; cakes and biscuits),offer mainly wholemeal carbohydrates (whole-grain bread; brown rice; or pasta for example),offer only high quality grass-fed meat options</t>
         </is>
       </c>
       <c r="BG66" t="n">
@@ -18205,7 +18205,7 @@
       </c>
       <c r="BH66" t="inlineStr">
         <is>
-          <t>reduce high-carbon &amp; water footprint foods (meat and dairy, for example),minimise waste,contain locally sourced ingredients,contain organically sourced ingredients,contain  seasonally sourced ingredients,are cooked from scratch in the school kitchen,meet all dietary requirements,should be enjoyed by pupils,offer high quality grass-fed meat options</t>
+          <t>reduce high-carbon &amp; water footprint foods (meat and dairy; for example),minimise waste,contain locally sourced ingredients,contain organically sourced ingredients,contain  seasonally sourced ingredients,are cooked from scratch in the school kitchen,meet all dietary requirements,should be enjoyed by pupils,offer high quality grass-fed meat options</t>
         </is>
       </c>
       <c r="BJ66" t="n">
@@ -18338,10 +18338,10 @@
         </is>
       </c>
       <c r="N67" t="n">
-        <v>33.19549560546875</v>
+        <v>33.1954956054687</v>
       </c>
       <c r="O67" t="n">
-        <v>-117.2862014770508</v>
+        <v>-117.286201477051</v>
       </c>
       <c r="P67" t="inlineStr">
         <is>
@@ -18415,12 +18415,12 @@
       </c>
       <c r="BE67" t="inlineStr">
         <is>
-          <t>offer at least one portion of fresh fruit and vegetables everyday,are void of trans-fats* (artificially created fats used in the manufacture of foods to increase shelf life and the flavour-stability of foods. They are also often found in fast food, margarine, cakes and biscuits),offer mainly wholemeal carbohydrates (whole-grain bread, brown rice, or pasta for example)</t>
+          <t>offer at least one portion of fresh fruit and vegetables everyday,are void of trans-fats* (artificially created fats used in the manufacture of foods to increase shelf life and the flavour-stability of foods. They are also often found in fast food; margarine; cakes and biscuits),offer mainly wholemeal carbohydrates (whole-grain bread; brown rice; or pasta for example)</t>
         </is>
       </c>
       <c r="BH67" t="inlineStr">
         <is>
-          <t>reduce high-carbon &amp; water footprint foods (meat and dairy, for example),minimise waste,contain locally sourced ingredients,meet all dietary requirements,should be enjoyed by pupils</t>
+          <t>reduce high-carbon &amp; water footprint foods (meat and dairy; for example),minimise waste,contain locally sourced ingredients,meet all dietary requirements,should be enjoyed by pupils</t>
         </is>
       </c>
       <c r="BK67" t="inlineStr">
@@ -18629,7 +18629,7 @@
       </c>
       <c r="BH68" t="inlineStr">
         <is>
-          <t>reduce high-carbon &amp; water footprint foods (meat and dairy, for example),contain locally sourced ingredients,should be enjoyed by pupils</t>
+          <t>reduce high-carbon &amp; water footprint foods (meat and dairy; for example),contain locally sourced ingredients,should be enjoyed by pupils</t>
         </is>
       </c>
       <c r="BJ68" t="n">
@@ -18856,7 +18856,7 @@
       </c>
       <c r="BE70" t="inlineStr">
         <is>
-          <t>offer at least one portion of fresh fruit and vegetables everyday,are void of trans-fats* (artificially created fats used in the manufacture of foods to increase shelf life and the flavour-stability of foods. They are also often found in fast food, margarine, cakes and biscuits),offer mainly wholemeal carbohydrates (whole-grain bread, brown rice, or pasta for example),offer only high quality grass-fed meat options</t>
+          <t>offer at least one portion of fresh fruit and vegetables everyday,are void of trans-fats* (artificially created fats used in the manufacture of foods to increase shelf life and the flavour-stability of foods. They are also often found in fast food; margarine; cakes and biscuits),offer mainly wholemeal carbohydrates (whole-grain bread; brown rice; or pasta for example),offer only high quality grass-fed meat options</t>
         </is>
       </c>
       <c r="BG70" t="n">
@@ -18864,7 +18864,7 @@
       </c>
       <c r="BH70" t="inlineStr">
         <is>
-          <t>reduce high-carbon &amp; water footprint foods (meat and dairy, for example),minimise waste,contain locally sourced ingredients,contain  seasonally sourced ingredients,should be enjoyed by pupils</t>
+          <t>reduce high-carbon &amp; water footprint foods (meat and dairy; for example),minimise waste,contain locally sourced ingredients,contain  seasonally sourced ingredients,should be enjoyed by pupils</t>
         </is>
       </c>
       <c r="BJ70" t="n">
@@ -19473,7 +19473,7 @@
       </c>
       <c r="BE73" t="inlineStr">
         <is>
-          <t>offer at least one portion of fresh fruit and vegetables everyday,offer fruit only, or fruit-based puddings,are void of trans-fats* (artificially created fats used in the manufacture of foods to increase shelf life and the flavour-stability of foods. They are also often found in fast food, margarine, cakes and biscuits),offer mainly wholemeal carbohydrates (whole-grain bread, brown rice, or pasta for example)</t>
+          <t>offer at least one portion of fresh fruit and vegetables everyday,offer fruit only, or fruit-based puddings,are void of trans-fats* (artificially created fats used in the manufacture of foods to increase shelf life and the flavour-stability of foods. They are also often found in fast food; margarine; cakes and biscuits),offer mainly wholemeal carbohydrates (whole-grain bread; brown rice; or pasta for example)</t>
         </is>
       </c>
       <c r="BG73" t="n">
@@ -19481,7 +19481,7 @@
       </c>
       <c r="BH73" t="inlineStr">
         <is>
-          <t>reduce high-carbon &amp; water footprint foods (meat and dairy, for example),minimise waste,contain locally sourced ingredients,contain  seasonally sourced ingredients,are cooked from scratch in the school kitchen,should be enjoyed by pupils</t>
+          <t>reduce high-carbon &amp; water footprint foods (meat and dairy; for example),minimise waste,contain locally sourced ingredients,contain  seasonally sourced ingredients,are cooked from scratch in the school kitchen,should be enjoyed by pupils</t>
         </is>
       </c>
       <c r="BJ73" t="n">
@@ -19680,7 +19680,7 @@
       </c>
       <c r="BE74" t="inlineStr">
         <is>
-          <t>offer at least one portion of fresh fruit and vegetables everyday,are void of trans-fats* (artificially created fats used in the manufacture of foods to increase shelf life and the flavour-stability of foods. They are also often found in fast food, margarine, cakes and biscuits),offer only high quality grass-fed meat options</t>
+          <t>offer at least one portion of fresh fruit and vegetables everyday,are void of trans-fats* (artificially created fats used in the manufacture of foods to increase shelf life and the flavour-stability of foods. They are also often found in fast food; margarine; cakes and biscuits),offer only high quality grass-fed meat options</t>
         </is>
       </c>
       <c r="BG74" t="n">
@@ -19688,7 +19688,7 @@
       </c>
       <c r="BH74" t="inlineStr">
         <is>
-          <t>reduce high-carbon &amp; water footprint foods (meat and dairy, for example),minimise waste,contain locally sourced ingredients,should be enjoyed by pupils</t>
+          <t>reduce high-carbon &amp; water footprint foods (meat and dairy; for example),minimise waste,contain locally sourced ingredients,should be enjoyed by pupils</t>
         </is>
       </c>
       <c r="BJ74" t="n">
@@ -19926,10 +19926,10 @@
         </is>
       </c>
       <c r="N77" t="n">
-        <v>51.61439514160156</v>
+        <v>51.6143951416016</v>
       </c>
       <c r="O77" t="n">
-        <v>-0.3368072509765625</v>
+        <v>-0.336807250976562</v>
       </c>
       <c r="P77" t="inlineStr">
         <is>
@@ -20008,7 +20008,7 @@
       </c>
       <c r="BE77" t="inlineStr">
         <is>
-          <t>offer at least one portion of fresh fruit and vegetables everyday,are void of trans-fats* (artificially created fats used in the manufacture of foods to increase shelf life and the flavour-stability of foods. They are also often found in fast food, margarine, cakes and biscuits),offer added-sugar free days,offer mainly wholemeal carbohydrates (whole-grain bread, brown rice, or pasta for example)</t>
+          <t>offer at least one portion of fresh fruit and vegetables everyday,are void of trans-fats* (artificially created fats used in the manufacture of foods to increase shelf life and the flavour-stability of foods. They are also often found in fast food; margarine; cakes and biscuits),offer added-sugar free days,offer mainly wholemeal carbohydrates (whole-grain bread; brown rice; or pasta for example)</t>
         </is>
       </c>
       <c r="BG77" t="n">
@@ -20261,10 +20261,10 @@
         </is>
       </c>
       <c r="N79" t="n">
-        <v>50.73739624023438</v>
+        <v>50.7373962402344</v>
       </c>
       <c r="O79" t="n">
-        <v>-3.470794677734375</v>
+        <v>-3.47079467773437</v>
       </c>
       <c r="P79" t="inlineStr">
         <is>
@@ -20341,7 +20341,7 @@
       </c>
       <c r="BH79" t="inlineStr">
         <is>
-          <t>reduce high-carbon &amp; water footprint foods (meat and dairy, for example),contain locally sourced ingredients,contain  seasonally sourced ingredients,are cooked from scratch in the school kitchen,should be enjoyed by pupils</t>
+          <t>reduce high-carbon &amp; water footprint foods (meat and dairy; for example),contain locally sourced ingredients,contain  seasonally sourced ingredients,are cooked from scratch in the school kitchen,should be enjoyed by pupils</t>
         </is>
       </c>
       <c r="BJ79" t="n">
@@ -20644,17 +20644,17 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>offer mainly wholemeal carbohydrates (whole-grain bread</t>
+          <t>offer at least one portion of fresh fruit and vegetables everyday</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>33</v>
+        <v>60</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>brown rice</t>
+          <t>offer mainly wholemeal carbohydrates (whole-grain bread; brown rice; or pasta for example)</t>
         </is>
       </c>
       <c r="B3" t="n">
@@ -20664,7 +20664,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>margarine</t>
+          <t>are void of trans-fats* (artificially created fats used in the manufacture of foods to increase shelf life and the flavour-stability of foods. They are also often found in fast food; margarine; cakes and biscuits)</t>
         </is>
       </c>
       <c r="B4" t="n">
@@ -20674,71 +20674,71 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>are void of trans-fats* (artificially created fats used in the manufacture of foods to increase shelf life and the flavour-stability of foods. They are also often found in fast food</t>
+          <t>offer only high quality grass-fed meat options</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>28</v>
+        <v>24</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>cakes and biscuits)</t>
+          <t>offer added-sugar free days</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>27</v>
+        <v>16</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>or pasta for example)</t>
+          <t>nan</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>19</v>
+        <v>14</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>offer only high quality grass-fed meat options offer at least one portion of fresh fruit and vegetables everyday</t>
+          <t>offer fruit only</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>offer added-sugar free days</t>
+          <t>or fruit-based puddings</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>or pasta for example) offer at least one portion of fresh fruit and vegetables everyday</t>
+          <t>Other</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>offer fruit only</t>
+          <t>please specify below:</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>
@@ -20779,37 +20779,37 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>50</v>
+        <v>55</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>contain  seasonally sourced ingredients</t>
+          <t>minimise waste</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>42</v>
+        <v>53</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>for example)</t>
+          <t>should be enjoyed by pupils</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>36</v>
+        <v>53</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>meet all dietary requirements</t>
+          <t>contain  seasonally sourced ingredients</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>33</v>
+        <v>43</v>
       </c>
     </row>
     <row r="6">
@@ -20819,57 +20819,57 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>33</v>
+        <v>37</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>minimise waste</t>
+          <t>meet all dietary requirements</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>32</v>
+        <v>36</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>contain organically sourced ingredients</t>
+          <t>reduce high-carbon &amp; water footprint foods (meat and dairy; for example)</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>21</v>
+        <v>36</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>should be enjoyed by pupils reduce high-carbon &amp; water footprint foods (meat and dairy</t>
+          <t>contain organically sourced ingredients</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>18</v>
+        <v>21</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>should be enjoyed by pupils</t>
+          <t>offer high quality grass-fed meat options</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>offer high quality grass-fed meat options reduce high-carbon &amp; water footprint foods (meat and dairy</t>
+          <t>nan</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>8</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>